<commit_message>
fix: directory path for saving images
</commit_message>
<xml_diff>
--- a/server/book data.xlsx
+++ b/server/book data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9981B0-E6C2-425B-8A47-0200AB06885D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0D165A-B720-448E-894E-5DE84C2890B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,7 +453,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{BF14E51E-706C-4F95-9EED-715A30904AF9}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{7175BDAE-8490-4318-BC8E-1E5674BFABBF}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -732,7 +732,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
fix: save data with correct data types
</commit_message>
<xml_diff>
--- a/server/book data.xlsx
+++ b/server/book data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0D165A-B720-448E-894E-5DE84C2890B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4489D0F1-1C91-4FEA-9786-21F08458414B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="117">
   <si>
     <t>id</t>
   </si>
@@ -405,6 +405,17 @@
   </si>
   <si>
     <t>29 The Girls We Sent Away.jpg</t>
+  </si>
+  <si>
+    <t>Den of Thieves</t>
+  </si>
+  <si>
+    <t>A #1 bestseller from coast to coast, Den of Thieves tells the full story of the insider-trading scandal that nearly destroyed Wall Street, the men who pulled it off, and the chase that finally brought them to justice.
+Pulitzer Prize-winner James B. Stewart shows for the first time how four of the eighties' biggest names on Wall Street--Michael Milken, Ivan Boesky, Martin Siegel, and Dennis Levine--created the greatest insider-trading ring in financial history and almost walked away with billions, until a team of downtrodden detectives triumphed over some of America's most expensive lawyers to bring this powerful quartet to justice.
+Based on secret grand jury transcripts, interviews, and actual trading records, and containing explosive new revelations about Michael Milken and Ivan Boesky, Den of Thieves weaves all the facts into an unforgettable narrative--a portrait of human nature, big business, and crime of unparalleled proportions.</t>
+  </si>
+  <si>
+    <t>30 Den of Thieves.jpg</t>
   </si>
 </sst>
 </file>
@@ -440,20 +451,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{7175BDAE-8490-4318-BC8E-1E5674BFABBF}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{7E6837DF-7D47-4E93-A673-A8EDE9306540}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -729,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1371,6 +1383,26 @@
         <v>45546</v>
       </c>
     </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" t="s">
+        <v>116</v>
+      </c>
+      <c r="F31" s="3">
+        <v>45560</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>